<commit_message>
sensor as per new extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A8:D24"/>
+  <oleSize ref="A15:D31"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="72">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>ZestIOT_016_Celebi_User_BFL_group_Activity_Validation</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com, pdwadasi@enhops.com, rchiluka@enhops.com, rbuddha@enhops.com, smunnangi@enhops.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZestIOT_018_GMR_HYD_Sensor_And_Scheduled_data_Validation </t>
   </si>
 </sst>
 </file>
@@ -644,7 +650,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,7 +788,9 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -815,10 +823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,6 +1049,14 @@
       </c>
       <c r="B21" s="6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cobt and sensor testcases added to jenkins pipeline
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="75">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -230,6 +230,24 @@
   </si>
   <si>
     <t>ZestIOT_018_GMR_HYD_Sensor_And_Scheduled_data_Validation</t>
+  </si>
+  <si>
+    <t>ZestIOT_2268_Verifying_COBT_For_DIALCelebi_User</t>
+  </si>
+  <si>
+    <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_AISATS_User</t>
+  </si>
+  <si>
+    <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_SG_User</t>
+  </si>
+  <si>
+    <t>ZestIOT_2293_GMR_HYD_Sensor_And_Scheduled_data_Validation</t>
+  </si>
+  <si>
+    <t>ZestIOT_2294_GMR_HYD_SensorATD_And_Scheduled_data_Validation</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -641,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +798,9 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -807,16 +827,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1026,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
@@ -1011,7 +1034,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
@@ -1019,7 +1042,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>10</v>
@@ -1027,9 +1050,17 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
code pushed by padmaja on 5th evng
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZestIOT\src\test\resources\ExcelFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -19,11 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A22:C39"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -229,9 +225,6 @@
     <t>ZestIOT_016_Celebi_User_BFL_group_Activity_Validation</t>
   </si>
   <si>
-    <t>ZestIOT_018_GMR_HYD_Sensor_And_Scheduled_data_Validation</t>
-  </si>
-  <si>
     <t>ZestIOT_2268_Verifying_COBT_For_DIALCelebi_User</t>
   </si>
   <si>
@@ -241,16 +234,16 @@
     <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_SG_User</t>
   </si>
   <si>
-    <t>ZestIOT_2293_GMR_HYD_Sensor_And_Scheduled_data_Validation</t>
-  </si>
-  <si>
-    <t>ZestIOT_2294_GMR_HYD_SensorATD_And_Scheduled_data_Validation</t>
-  </si>
-  <si>
     <t xml:space="preserve"> anantwar@zestiot.io, pdwadasi@enhops.com, rbuddha@enhops.com, smunnangi@enhops.com, mpyla@enhops.com, rchiluka@enhops.com, stiyyagura@enhops.com</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
+    <t>ZestIOT_AV_2293_GMR_HYD_SensorATA_And_Scheduled_data_Validation</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2294_GMR_HYD_SensorATD_And_Scheduled_data_Validation</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com, pdwadasi@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -361,7 +354,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -375,6 +368,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -662,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +798,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -831,7 +827,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -841,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1025,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
@@ -1037,7 +1033,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
@@ -1045,22 +1041,22 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1074,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A20" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1289,11 +1285,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>68</v>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1307,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,11 +1523,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>68</v>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sensor test cases parameter change to String from Int
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16065" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A22:C39"/>
+  <oleSize ref="A19:M24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -234,16 +234,13 @@
     <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_SG_User</t>
   </si>
   <si>
-    <t xml:space="preserve"> anantwar@zestiot.io, pdwadasi@enhops.com, rbuddha@enhops.com, smunnangi@enhops.com, mpyla@enhops.com, rchiluka@enhops.com, stiyyagura@enhops.com</t>
-  </si>
-  <si>
     <t>ZestIOT_AV_2293_GMR_HYD_SensorATA_And_Scheduled_data_Validation</t>
   </si>
   <si>
     <t>ZestIOT_AV_2294_GMR_HYD_SensorATD_And_Scheduled_data_Validation</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com, pdwadasi@enhops.com</t>
+    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -658,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,9 +794,7 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -826,9 +821,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -837,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1041,7 @@
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
@@ -1057,7 +1049,7 @@
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
@@ -1073,7 +1065,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,9 +1257,7 @@
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1287,7 +1277,7 @@
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
@@ -1295,16 +1285,13 @@
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1313,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B21"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,15 +1486,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1515,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1523,17 +1513,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>73</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
@@ -1541,6 +1531,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
removed emails from control sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16065" windowHeight="6015" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10560" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A12:E22"/>
+  <oleSize ref="A19:G24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -655,7 +655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -790,13 +790,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -823,9 +821,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1305,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
2307 test cases added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10560" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A19:G24"/>
+  <oleSize ref="A8:C23"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="75">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2307_GMR_HYD_SensorATA_OnBlock_OffBlock_SensorATD_Validation</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -827,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,6 +1055,14 @@
         <v>72</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test case name updated as per documentation
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A19:M31"/>
+  <oleSize ref="A22:C39"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -225,15 +225,6 @@
     <t>ZestIOT_016_Celebi_User_BFL_group_Activity_Validation</t>
   </si>
   <si>
-    <t>ZestIOT_2268_Verifying_COBT_For_DIALCelebi_User</t>
-  </si>
-  <si>
-    <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_AISATS_User</t>
-  </si>
-  <si>
-    <t>ZestIOT_2268_Verifying_COBT_For_GMR_HYD_SG_User</t>
-  </si>
-  <si>
     <t>ZestIOT_AV_2293_GMR_HYD_SensorATA_And_Scheduled_data_Validation</t>
   </si>
   <si>
@@ -243,10 +234,28 @@
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com</t>
   </si>
   <si>
-    <t>ZestIOT_AV_2307_GMR_HYD_SensorATA_OnBlock_OffBlock_SensorATD_Validation</t>
-  </si>
-  <si>
     <t>nishanth@zestiot.io, hmanthena@enhops.com, pdwadasi@enhops.com</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_DIALCelebi_User</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_GMR_HYD_AISATS_User</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_GMR_HYD_SG_User</t>
+  </si>
+  <si>
+    <t>AV_2293_Identify_coverage_of_Flight_Sensor_and_Validate_timestamps_of_Arrival_Aircrafts</t>
+  </si>
+  <si>
+    <t>AV_2294_Identify_coverage_of_Flight_Sensor_and_Validate_timestamps_of_Departure_Aircrafts</t>
+  </si>
+  <si>
+    <t>AV_2307_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>AV_2304_Identify_the_coverage_of_Boarding_activities_and_validate_timestamps</t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -801,7 +810,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,10 +844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +1034,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
@@ -1033,7 +1042,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
@@ -1041,23 +1050,23 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
@@ -1065,10 +1074,18 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1310,7 @@
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
@@ -1301,7 +1318,7 @@
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
@@ -1510,7 +1527,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1548,7 @@
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
@@ -1539,7 +1556,7 @@
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
mails updated in controlsheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A22:C39"/>
+  <oleSize ref="A19:M24"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="85">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -234,9 +234,6 @@
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
-  </si>
-  <si>
     <t>ZestIOT_AV_2268_Validate_Accuracy_of_COBT_For_DIALCelebi_User</t>
   </si>
   <si>
@@ -256,6 +253,27 @@
   </si>
   <si>
     <t>ZestIOT_AV_2304_Identify_the_coverage_of_Boarding_activities_and_validate_timestamps</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_DIALCelebi_User</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_GMR_HYD_AISATS_User</t>
+  </si>
+  <si>
+    <t>AV_2268_Validate_Accuracy_of_COBT_For_GMR_HYD_SG_User</t>
+  </si>
+  <si>
+    <t>AV_2293_Identify_coverage_of_Flight_Sensor_and_Validate_timestamps_of_Arrival_Aircrafts</t>
+  </si>
+  <si>
+    <t>AV_2294_Identify_coverage_of_Flight_Sensor_and_Validate_timestamps_of_Departure_Aircrafts</t>
+  </si>
+  <si>
+    <t>AV_2307_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>AV_2304_Identify_the_coverage_of_Boarding_activities_and_validate_timestamps</t>
   </si>
 </sst>
 </file>
@@ -366,7 +384,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -383,9 +401,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,12 +823,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>71</v>
+      <c r="B25" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -842,7 +857,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -852,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,60 +1053,81 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>78</v>
-      </c>
       <c r="B23" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1104,7 +1140,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mails removed in controlsheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -276,7 +276,7 @@
     <t>AV_2304_Identify_the_coverage_of_Boarding_activities_and_validate_timestamps</t>
   </si>
   <si>
-    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com,mpyla@enhops.com</t>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -404,6 +404,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,11 +829,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -860,7 +863,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
+    <hyperlink ref="B25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sensor ATA for Delhi with Test case pushed
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -276,13 +276,13 @@
     <t>AV_2304_Identify_the_coverage_of_Boarding_activities_and_validate_timestamps</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
+    <t>xxx@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -694,16 +694,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -728,7 +728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -745,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -762,7 +762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -779,12 +779,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -792,7 +792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -800,7 +800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -808,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -816,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -824,12 +824,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -837,7 +837,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -845,7 +845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -853,7 +853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -877,13 +877,13 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -894,7 +894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -905,7 +905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -916,7 +916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -927,7 +927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -938,7 +938,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -949,7 +949,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -960,7 +960,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -971,7 +971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -982,7 +982,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -993,7 +993,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>75</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1149,13 +1149,13 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1385,13 +1385,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1624,17 +1624,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
mails updated in control sheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A16:K31"/>
+  <oleSize ref="B12:G22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="79">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -231,9 +231,6 @@
     <t>ZestIOT_AV_2294_GMR_HYD_SensorATD_And_Scheduled_data_Validation</t>
   </si>
   <si>
-    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com</t>
-  </si>
-  <si>
     <t>ZestIOT_AV_2268_Validate_Accuracy_of_COBT_For_DIALCelebi_User</t>
   </si>
   <si>
@@ -258,7 +255,7 @@
     <t>ZestIOT_AV_2294__GMR_HYD_Identify_coverage_of_Flight_Sensor_and_Validate_timestamps_of_Departure_Aircrafts</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
+    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -369,7 +366,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -386,9 +383,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,12 +805,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>79</v>
+      <c r="B25" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +839,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1043,90 +1037,90 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1374,7 +1368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1568,7 +1562,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,8 +1598,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" display="stiyyagura@enhops.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
11th day mails removed from controlsheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="B12:G22"/>
+  <oleSize ref="A25:K25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="79">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,13 +805,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -838,9 +836,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1368,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+    <sheetView topLeftCell="B12" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new class created for send mail
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="80">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -383,6 +386,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,11 +811,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -836,6 +844,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
2307 for Delhi added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18012" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="80">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -256,12 +256,15 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
+  </si>
+  <si>
+    <t>xxx@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -383,6 +386,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,16 +676,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -704,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -721,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -738,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -755,12 +761,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -768,7 +774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -776,7 +782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -784,7 +790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -792,7 +798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -800,18 +806,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -819,7 +827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -827,7 +835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -836,6 +844,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -848,13 +859,13 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -865,7 +876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -876,7 +887,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -887,7 +898,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -898,7 +909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -909,7 +920,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -920,7 +931,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -931,7 +942,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -942,7 +953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -953,7 +964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -964,7 +975,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -975,7 +986,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -986,7 +997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -997,7 +1008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -1008,7 +1019,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1019,7 +1030,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1030,7 +1041,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1041,7 +1052,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1052,7 +1063,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1063,7 +1074,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
@@ -1074,7 +1085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>75</v>
       </c>
@@ -1085,7 +1096,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1096,7 +1107,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1107,7 +1118,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -1131,13 +1142,13 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1148,7 +1159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1159,7 +1170,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1170,7 +1181,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1181,7 +1192,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1192,7 +1203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1203,7 +1214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1214,7 +1225,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1225,7 +1236,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1236,7 +1247,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1247,7 +1258,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1258,7 +1269,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1269,7 +1280,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1280,7 +1291,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1291,7 +1302,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1302,7 +1313,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1313,7 +1324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1322,7 +1333,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1330,7 +1341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1338,7 +1349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1346,7 +1357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1367,13 +1378,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1406,7 +1417,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1417,7 +1428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1428,7 +1439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1439,7 +1450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1472,7 +1483,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1483,7 +1494,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1494,7 +1505,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1505,7 +1516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1516,7 +1527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1527,7 +1538,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1538,7 +1549,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1549,7 +1560,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1560,7 +1571,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1576,7 +1587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1584,7 +1595,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1609,17 +1620,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
colour code changed for headders
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A25:K25"/>
+  <oleSize ref="A15:C28"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -259,12 +259,18 @@
   </si>
   <si>
     <t>stiyyagura@enhops.com</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2307_DIAL_Delhi_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2307_GMR_HYD_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -676,16 +682,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F33:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -710,7 +716,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -727,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -744,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -761,12 +767,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -774,7 +780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -782,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -790,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -798,7 +804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -806,12 +812,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -819,7 +825,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -827,7 +833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -835,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -853,19 +859,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -876,7 +882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -887,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -898,7 +904,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -909,7 +915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -920,7 +926,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -931,7 +937,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -942,7 +948,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -953,7 +959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -964,7 +970,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -975,7 +981,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -986,7 +992,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1052,7 +1058,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
@@ -1085,7 +1091,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>75</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1118,15 +1124,26 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1142,13 +1159,13 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1159,7 +1176,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1170,7 +1187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1181,7 +1198,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1192,7 +1209,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1203,7 +1220,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1214,7 +1231,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1225,7 +1242,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1236,7 +1253,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1247,7 +1264,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1258,7 +1275,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1269,7 +1286,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1280,7 +1297,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1291,7 +1308,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1302,7 +1319,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1313,7 +1330,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1324,7 +1341,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1333,7 +1350,7 @@
       </c>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1341,7 +1358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1349,7 +1366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1357,7 +1374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1378,13 +1395,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1412,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -1406,7 +1423,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1417,7 +1434,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>34</v>
       </c>
@@ -1428,7 +1445,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -1439,7 +1456,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1450,7 +1467,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -1461,7 +1478,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1472,7 +1489,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1483,7 +1500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -1494,7 +1511,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -1505,7 +1522,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -1516,7 +1533,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1527,7 +1544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1538,7 +1555,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -1549,7 +1566,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -1560,7 +1577,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1571,7 +1588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -1579,7 +1596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1587,7 +1604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
@@ -1595,7 +1612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>69</v>
       </c>
@@ -1620,17 +1637,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
mails updated in jenkins and control sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A15:C28"/>
+  <oleSize ref="A12:L29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>ZestIOT_AV_2307_GMR_HYD_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
-  </si>
-  <si>
-    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -375,7 +372,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -392,9 +389,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -682,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,12 +811,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>81</v>
+      <c r="B25" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +845,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -861,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B25"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1057,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
@@ -1074,7 +1068,7 @@
         <v>72</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -1085,7 +1079,7 @@
         <v>74</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>74</v>
@@ -1096,7 +1090,7 @@
         <v>75</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>75</v>
@@ -1107,7 +1101,7 @@
         <v>76</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -1118,7 +1112,7 @@
         <v>77</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -1129,7 +1123,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>73</v>
@@ -1140,7 +1134,7 @@
         <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
mails removed in jenkins and control sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\git\ZestIOTAutomation\src\test\resources\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015"/>
   </bookViews>
@@ -14,12 +19,11 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A12:L29"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="81">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -372,7 +376,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -389,6 +393,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,177 +683,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.85546875" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -856,7 +859,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
email code updated jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>ZestIOT_AV_2307_GMR_HYD_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>Script_Reference</t>
   </si>
 </sst>
 </file>
@@ -376,7 +379,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -396,6 +399,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -683,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -824,6 +830,7 @@
       <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -856,10 +863,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +877,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
@@ -1060,7 +1067,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
@@ -1071,7 +1078,7 @@
         <v>72</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -1082,7 +1089,7 @@
         <v>74</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>74</v>
@@ -1093,7 +1100,7 @@
         <v>75</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>75</v>
@@ -1104,7 +1111,7 @@
         <v>76</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -1115,7 +1122,7 @@
         <v>77</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -1126,7 +1133,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>73</v>
@@ -1137,11 +1144,17 @@
         <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>
       </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
borading activities code added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="6015"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="83">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Script_Reference</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -689,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +833,9 @@
       <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
+      <c r="B25" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -857,6 +862,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -865,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1075,7 @@
         <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
@@ -1078,7 +1086,7 @@
         <v>72</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -1089,7 +1097,7 @@
         <v>74</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>74</v>
@@ -1100,7 +1108,7 @@
         <v>75</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>75</v>
@@ -1111,7 +1119,7 @@
         <v>76</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -1122,7 +1130,7 @@
         <v>77</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -1133,7 +1141,7 @@
         <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
         <v>73</v>
@@ -1144,7 +1152,7 @@
         <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
mails added in jenkins file and control sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -269,9 +269,6 @@
   </si>
   <si>
     <t>Script_Reference</t>
-  </si>
-  <si>
-    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -382,7 +379,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -402,9 +399,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,7 +687,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,8 +827,8 @@
       <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>82</v>
+      <c r="B25" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +857,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
+    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
colour removed in pages
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -868,7 +868,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1146,7 @@
         <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
mails removed from control sheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -827,9 +827,6 @@
       <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -856,9 +853,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
mails removed in control sheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="6015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="6015" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="44">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -152,13 +152,16 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -199,6 +202,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -222,20 +233,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -518,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,12 +668,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="132" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>42</v>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,8 +701,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -827,7 +844,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +973,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,6 +1092,11 @@
         <v>41</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="99" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
@@ -1087,7 +1109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test output also updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\padmaja\git\ZestIOTAutomation\src\test\resources\ExcelFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="6720" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16296" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -14,12 +19,11 @@
     <sheet name="DeviceName" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O21"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="52">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -169,6 +173,9 @@
   </si>
   <si>
     <t>ZestIOT_AV_2307_GMR_HYD_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2268_Validate_Accuracy_of_COBT_For_DIALCelebi_User</t>
   </si>
   <si>
     <t>pdwadasi@enhops.com</t>
@@ -592,7 +599,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +738,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -768,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,10 +800,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>41</v>
@@ -807,7 +814,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>42</v>
@@ -818,7 +825,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>43</v>
@@ -829,7 +836,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>44</v>
@@ -840,7 +847,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>45</v>
@@ -851,7 +858,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>46</v>
@@ -862,7 +869,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>47</v>
@@ -873,7 +880,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>48</v>
@@ -883,8 +890,8 @@
       <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>49</v>
@@ -892,12 +899,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -945,7 +952,6 @@
       <c r="B21" s="11"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -955,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1321,7 +1327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test case report updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -632,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +850,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>42</v>
@@ -861,7 +861,7 @@
         <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>43</v>
@@ -872,7 +872,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>44</v>
@@ -883,7 +883,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>45</v>
@@ -894,7 +894,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>46</v>
@@ -905,7 +905,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>47</v>
@@ -916,7 +916,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>48</v>
@@ -927,7 +927,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>49</v>
@@ -938,7 +938,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>51</v>
@@ -949,7 +949,7 @@
         <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>52</v>
@@ -960,7 +960,7 @@
         <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>53</v>
@@ -971,7 +971,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>54</v>
@@ -982,7 +982,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>55</v>
@@ -993,7 +993,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>56</v>
@@ -1004,7 +1004,7 @@
         <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>57</v>
@@ -1015,7 +1015,7 @@
         <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
mails added in control sheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -211,7 +211,7 @@
     <t>ZestIOT_015_Celebi_User_Pushback_group_Activity_Validation</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
+    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com, dbandi@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -247,12 +247,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color indexed="8"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -316,11 +314,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -344,12 +341,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -632,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +764,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="264" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -801,11 +797,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -813,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
latest code up to 23rd dec
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="81">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -211,14 +211,68 @@
     <t>ZestIOT_015_Celebi_User_Pushback_group_Activity_Validation</t>
   </si>
   <si>
-    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com, dbandi@enhops.com</t>
+    <t>Executed For</t>
+  </si>
+  <si>
+    <t>Execution Type</t>
+  </si>
+  <si>
+    <t>TC.No.</t>
+  </si>
+  <si>
+    <t>Test Case name</t>
+  </si>
+  <si>
+    <t>AV 2268 Validate Accuracy of COBT</t>
+  </si>
+  <si>
+    <t>DIAL Celebi</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>GMR-HYD-AISATS</t>
+  </si>
+  <si>
+    <t>GMR-HYD-SG</t>
+  </si>
+  <si>
+    <t>AV 2307 Validate LANDING ONBLOCK OFFBLOCK AIRBORNE timestamps of Arrival and Departure aircrafts Any Data source</t>
+  </si>
+  <si>
+    <t>DIAL-Delhi</t>
+  </si>
+  <si>
+    <t>GMR-Hyd</t>
+  </si>
+  <si>
+    <t>AV 2293 Identify coverage of Flight Sensor and Validate timestamps of Arrival Aircrafts</t>
+  </si>
+  <si>
+    <t>BSSPL-Delhi</t>
+  </si>
+  <si>
+    <t>AISATS-Hyd</t>
+  </si>
+  <si>
+    <t>SG-Hyd</t>
+  </si>
+  <si>
+    <t>CELEBI-Delhi</t>
+  </si>
+  <si>
+    <t>AV 2294 Identify coverage of Flight Sensor and Validate timestamps of Departure Aircrafts</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -247,13 +301,68 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF201F1E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008AE6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +374,26 @@
         <fgColor indexed="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF80E5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -313,13 +440,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -338,14 +481,28 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -628,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,12 +921,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="264" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>62</v>
+      <c r="B25" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -797,258 +954,374 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="13"/>
+    <col min="3" max="3" width="78.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="16" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="D1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="B11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="B12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="B16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="B17" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="B18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1056,7 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -1420,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,14 +1704,266 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="363.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="363.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="248.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>14</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="264.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try catch added in jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
     <t>ZestIOT_000_bsspl</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
+    <t>xxx@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -866,7 +866,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>42</v>
@@ -1155,7 +1155,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
test cases updated in control sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="73">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -232,7 +232,16 @@
     <t>ZestIOT_000_bsspl</t>
   </si>
   <si>
-    <t>xxx@enhops.com</t>
+    <t>ZestIOT_AV_2307_UI_CELEBI_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
+  </si>
+  <si>
+    <t>ZestIOT_AV_2405_UI_BSSPL_Validate_Fueling_Coverage</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
@@ -649,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +698,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -706,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -790,7 +799,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1254,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>42</v>
@@ -1271,7 +1280,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1288,7 +1297,7 @@
         <v>38</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>47</v>
@@ -1305,7 +1314,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>47</v>
@@ -1322,7 +1331,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>50</v>
@@ -1339,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>50</v>
@@ -1356,7 +1365,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>50</v>
@@ -1373,7 +1382,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>50</v>
@@ -1390,7 +1399,7 @@
         <v>60</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>50</v>
@@ -1407,7 +1416,7 @@
         <v>61</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>50</v>
@@ -1424,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>55</v>
@@ -1441,7 +1450,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>55</v>
@@ -1458,7 +1467,7 @@
         <v>62</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>55</v>
@@ -1475,7 +1484,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>55</v>
@@ -1492,7 +1501,7 @@
         <v>64</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>55</v>
@@ -1509,7 +1518,7 @@
         <v>65</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>55</v>
@@ -1526,7 +1535,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>67</v>
@@ -1543,7 +1552,7 @@
         <v>66</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>47</v>
@@ -1555,8 +1564,39 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
+    <row r="21" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
mails added in controlsheet and jenkins file
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -247,9 +247,6 @@
     <t>AV_2268_COBT_For_DIALCelebi_User.email_COBT_For_DIALCelebi_User5</t>
   </si>
   <si>
-    <t>stiyyagura@enhops.com</t>
-  </si>
-  <si>
     <t>ZestIOT_AV_2307_UI_AISATS_HYD_Validate_LANDING_ONBLOCK_OFFBLOCK_AIRBORNE_timestamps_of_Arrival_and_Departure_aircrafts_Any_Data_source</t>
   </si>
   <si>
@@ -320,13 +317,16 @@
   </si>
   <si>
     <t>ZestIOT_AV_2390_UI_SG_HYD_Detect_totalNo_offlights_forwhich_finalCOBT_hashighOrless_difference_compareto_Actual_Offblock</t>
+  </si>
+  <si>
+    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -375,14 +375,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -427,13 +419,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,12 +448,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -745,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -881,12 +868,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>74</v>
+      <c r="B25" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -914,11 +901,8 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1693,7 +1677,7 @@
     </row>
     <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>7</v>
@@ -1710,7 +1694,7 @@
     </row>
     <row r="24" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -1727,7 +1711,7 @@
     </row>
     <row r="25" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>7</v>
@@ -1744,7 +1728,7 @@
     </row>
     <row r="26" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>7</v>
@@ -1753,7 +1737,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>71</v>
@@ -1761,7 +1745,7 @@
     </row>
     <row r="27" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>7</v>
@@ -1778,16 +1762,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>71</v>
@@ -1795,16 +1779,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>71</v>
@@ -1812,16 +1796,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>71</v>
@@ -1829,16 +1813,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>71</v>
@@ -1846,16 +1830,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>71</v>
@@ -1863,13 +1847,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>53</v>
@@ -1880,16 +1864,16 @@
     </row>
     <row r="34" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>71</v>
@@ -1897,13 +1881,13 @@
     </row>
     <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>51</v>
@@ -1914,13 +1898,13 @@
     </row>
     <row r="36" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>54</v>
@@ -1931,16 +1915,16 @@
     </row>
     <row r="37" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>71</v>
@@ -1948,16 +1932,16 @@
     </row>
     <row r="38" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>71</v>
@@ -1965,13 +1949,13 @@
     </row>
     <row r="39" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
path changed in all files
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="100">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -320,13 +320,16 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -375,6 +378,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -419,12 +430,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,8 +460,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -732,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,12 +884,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="148.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>98</v>
+      <c r="B25" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -901,8 +917,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -910,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -949,7 +968,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>42</v>
@@ -1241,7 +1260,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>67</v>
@@ -2344,8 +2363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
mails updated in control sheet and Cobt class updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
     <t>ZestIOT_AV_2390_UI_SG_HYD_Detect_totalNo_offlights_forwhich_finalCOBT_hashighOrless_difference_compareto_Actual_Offblock</t>
   </si>
   <si>
-    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com, venkatesh@zestiot.io</t>
+    <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com, venkatesh@zestiot.io, ravi@zestiot.io</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +914,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -972,7 +972,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>42</v>
@@ -989,7 +989,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2347,7 +2347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2361,7 +2361,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
cobt activity code finished
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="100">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -320,13 +320,16 @@
   </si>
   <si>
     <t>nilesh@zestiot.io, amit@zestiot.io, sushanto@zestiot.io, sudhir@zestiot.io, Krishna@zestiot.io, anantwar@zestiot.io, shrikant@zestiot.io, aman@zestiot.io, rohan@zestiot.io, leadership@enhops.com, chiranjeevi@zestiot.io, stiyyagura@enhops.com, pdwadasi@enhops.com, rbuddha@enhops.com, rchiluka@enhops.com, smunnangi@enhops.com, nishanth@zestiot.io, hmanthena@enhops.com, mpyla@enhops.com, venkatesh@zestiot.io, ravi@zestiot.io</t>
+  </si>
+  <si>
+    <t>stiyyagura@enhops.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -375,6 +378,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -419,12 +430,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -448,8 +460,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="1"/>
@@ -732,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -789,7 +805,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -868,12 +884,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>98</v>
+      <c r="B25" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -902,7 +918,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" display="stiyyagura@enhops.com"/>
+    <hyperlink ref="B25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -913,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -972,7 +988,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>42</v>
@@ -989,7 +1005,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>42</v>

</xml_diff>